<commit_message>
error base de datos corregido
</commit_message>
<xml_diff>
--- a/datos_from_py.xlsx
+++ b/datos_from_py.xlsx
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
@@ -2139,7 +2139,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
@@ -2491,7 +2491,7 @@
         </is>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
@@ -2541,7 +2541,7 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="n">
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="n">
@@ -2949,7 +2949,7 @@
         </is>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="n">
@@ -3049,7 +3049,7 @@
         </is>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="n">
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="n">
@@ -3301,7 +3301,7 @@
         </is>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="n">
@@ -3559,7 +3559,7 @@
         </is>
       </c>
       <c r="K61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="n">
@@ -3815,7 +3815,7 @@
         </is>
       </c>
       <c r="K66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L66" t="inlineStr"/>
       <c r="M66" t="n">
@@ -4275,7 +4275,7 @@
         </is>
       </c>
       <c r="K75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75" t="inlineStr"/>
       <c r="M75" t="n">
@@ -4325,7 +4325,7 @@
         </is>
       </c>
       <c r="K76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76" t="inlineStr"/>
       <c r="M76" t="n">
@@ -4479,7 +4479,7 @@
         </is>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" t="inlineStr"/>
       <c r="M79" t="n">
@@ -4529,7 +4529,7 @@
         </is>
       </c>
       <c r="K80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L80" t="inlineStr"/>
       <c r="M80" t="n">
@@ -4579,7 +4579,7 @@
         </is>
       </c>
       <c r="K81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" t="inlineStr"/>
       <c r="M81" t="n">
@@ -4629,7 +4629,7 @@
         </is>
       </c>
       <c r="K82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L82" t="inlineStr"/>
       <c r="M82" t="n">
@@ -4679,7 +4679,7 @@
         </is>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83" t="inlineStr"/>
       <c r="M83" t="n">
@@ -4781,7 +4781,7 @@
         </is>
       </c>
       <c r="K85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L85" t="inlineStr"/>
       <c r="M85" t="n">
@@ -4883,7 +4883,7 @@
         </is>
       </c>
       <c r="K87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L87" t="inlineStr"/>
       <c r="M87" t="n">
@@ -5037,7 +5037,7 @@
         </is>
       </c>
       <c r="K90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L90" t="inlineStr"/>
       <c r="M90" t="n">
@@ -5087,7 +5087,7 @@
         </is>
       </c>
       <c r="K91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L91" t="inlineStr"/>
       <c r="M91" t="n">
@@ -5293,7 +5293,7 @@
         </is>
       </c>
       <c r="K95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L95" t="inlineStr"/>
       <c r="M95" t="n">
@@ -5343,7 +5343,7 @@
         </is>
       </c>
       <c r="K96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" t="inlineStr"/>
       <c r="M96" t="n">
@@ -5393,7 +5393,7 @@
         </is>
       </c>
       <c r="K97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="n">
@@ -5443,7 +5443,7 @@
         </is>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L98" t="inlineStr"/>
       <c r="M98" t="n">
@@ -5801,7 +5801,7 @@
         </is>
       </c>
       <c r="K105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L105" t="inlineStr"/>
       <c r="M105" t="n">
@@ -5851,7 +5851,7 @@
         </is>
       </c>
       <c r="K106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L106" t="inlineStr"/>
       <c r="M106" t="n">
@@ -5901,7 +5901,7 @@
         </is>
       </c>
       <c r="K107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L107" t="inlineStr"/>
       <c r="M107" t="n">
@@ -6053,7 +6053,7 @@
         </is>
       </c>
       <c r="K110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="n">
@@ -6155,7 +6155,7 @@
         </is>
       </c>
       <c r="K112" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L112" t="inlineStr"/>
       <c r="M112" t="n">
@@ -6205,7 +6205,7 @@
         </is>
       </c>
       <c r="K113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L113" t="inlineStr"/>
       <c r="M113" t="n">
@@ -6255,7 +6255,7 @@
         </is>
       </c>
       <c r="K114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L114" t="inlineStr"/>
       <c r="M114" t="n">
@@ -6357,7 +6357,7 @@
         </is>
       </c>
       <c r="K116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L116" t="inlineStr"/>
       <c r="M116" t="n">
@@ -6405,7 +6405,7 @@
         </is>
       </c>
       <c r="K117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L117" t="inlineStr"/>
       <c r="M117" t="n">
@@ -6557,7 +6557,7 @@
         </is>
       </c>
       <c r="K120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L120" t="inlineStr"/>
       <c r="M120" t="n">
@@ -7947,7 +7947,7 @@
         </is>
       </c>
       <c r="K147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L147" t="inlineStr"/>
       <c r="M147" t="n">
@@ -8101,7 +8101,7 @@
         </is>
       </c>
       <c r="K150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L150" t="inlineStr"/>
       <c r="M150" t="n">
@@ -9173,7 +9173,7 @@
         </is>
       </c>
       <c r="K171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L171" t="inlineStr"/>
       <c r="M171" t="n">
@@ -10755,7 +10755,7 @@
         </is>
       </c>
       <c r="K202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L202" t="inlineStr"/>
       <c r="M202" t="n">
@@ -10909,7 +10909,7 @@
         </is>
       </c>
       <c r="K205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L205" t="inlineStr"/>
       <c r="M205" t="n">
@@ -11011,7 +11011,7 @@
         </is>
       </c>
       <c r="K207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L207" t="inlineStr"/>
       <c r="M207" t="n">
@@ -12141,7 +12141,7 @@
         </is>
       </c>
       <c r="K229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L229" t="inlineStr"/>
       <c r="M229" t="n">
@@ -12399,7 +12399,7 @@
         </is>
       </c>
       <c r="K234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L234" t="inlineStr"/>
       <c r="M234" t="n">

</xml_diff>